<commit_message>
Added Reti's numbers. LOL
</commit_message>
<xml_diff>
--- a/Arkansas_Data/Data/All_MI_measurements_empty.xlsx
+++ b/Arkansas_Data/Data/All_MI_measurements_empty.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhang\Documents\GitHub\Methane_Insight\Arkansas_Data\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9AFD494-48B5-4877-9395-C3F2F90C5621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0269BF0-378F-4699-B2F7-764F7C267D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1931" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2029" uniqueCount="227">
   <si>
     <t>Date</t>
   </si>
@@ -710,7 +710,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -723,13 +723,25 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -744,9 +756,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1046,8 +1063,8 @@
   <dimension ref="A1:F558"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+      <pane ySplit="1" topLeftCell="A284" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F301" sqref="F301:F312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,6 +1103,9 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
+      <c r="E2" s="2">
+        <v>37.69</v>
+      </c>
       <c r="F2" t="s">
         <v>204</v>
       </c>
@@ -1103,6 +1123,9 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
+      <c r="E3" s="2">
+        <v>-2.39</v>
+      </c>
       <c r="F3" t="s">
         <v>205</v>
       </c>
@@ -1120,6 +1143,9 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
+      <c r="E4" s="3">
+        <v>5.28</v>
+      </c>
       <c r="F4" t="s">
         <v>206</v>
       </c>
@@ -1137,6 +1163,9 @@
       <c r="D5" t="s">
         <v>8</v>
       </c>
+      <c r="E5" s="3">
+        <v>2.6</v>
+      </c>
       <c r="F5" t="s">
         <v>207</v>
       </c>
@@ -1154,6 +1183,9 @@
       <c r="D6" t="s">
         <v>7</v>
       </c>
+      <c r="E6" s="3">
+        <v>5.63</v>
+      </c>
       <c r="F6" t="s">
         <v>208</v>
       </c>
@@ -1171,6 +1203,9 @@
       <c r="D7" t="s">
         <v>8</v>
       </c>
+      <c r="E7" s="3">
+        <v>6.73</v>
+      </c>
       <c r="F7" t="s">
         <v>209</v>
       </c>
@@ -1188,6 +1223,9 @@
       <c r="D8" t="s">
         <v>7</v>
       </c>
+      <c r="E8" s="3">
+        <v>10.79</v>
+      </c>
       <c r="F8" t="s">
         <v>210</v>
       </c>
@@ -1205,6 +1243,9 @@
       <c r="D9" t="s">
         <v>8</v>
       </c>
+      <c r="E9" s="3">
+        <v>4.43</v>
+      </c>
       <c r="F9" t="s">
         <v>211</v>
       </c>
@@ -1222,6 +1263,9 @@
       <c r="D10" t="s">
         <v>7</v>
       </c>
+      <c r="E10" s="3">
+        <v>2.97</v>
+      </c>
       <c r="F10" t="s">
         <v>212</v>
       </c>
@@ -1239,6 +1283,9 @@
       <c r="D11" t="s">
         <v>8</v>
       </c>
+      <c r="E11" s="3">
+        <v>2.09</v>
+      </c>
       <c r="F11" t="s">
         <v>213</v>
       </c>
@@ -1256,6 +1303,9 @@
       <c r="D12" t="s">
         <v>7</v>
       </c>
+      <c r="E12" s="3">
+        <v>4.97</v>
+      </c>
       <c r="F12" t="s">
         <v>214</v>
       </c>
@@ -1273,6 +1323,9 @@
       <c r="D13" t="s">
         <v>8</v>
       </c>
+      <c r="E13" s="3">
+        <v>3.63</v>
+      </c>
       <c r="F13" t="s">
         <v>215</v>
       </c>
@@ -1290,6 +1343,9 @@
       <c r="D14" t="s">
         <v>7</v>
       </c>
+      <c r="E14" s="3">
+        <v>6.34</v>
+      </c>
       <c r="F14" t="s">
         <v>216</v>
       </c>
@@ -1307,6 +1363,9 @@
       <c r="D15" t="s">
         <v>8</v>
       </c>
+      <c r="E15" s="3">
+        <v>-0.88</v>
+      </c>
       <c r="F15" t="s">
         <v>217</v>
       </c>
@@ -1324,6 +1383,9 @@
       <c r="D16" t="s">
         <v>7</v>
       </c>
+      <c r="E16" s="3">
+        <v>28.59</v>
+      </c>
       <c r="F16" t="s">
         <v>218</v>
       </c>
@@ -1341,6 +1403,9 @@
       <c r="D17" t="s">
         <v>8</v>
       </c>
+      <c r="E17" s="3">
+        <v>4.84</v>
+      </c>
       <c r="F17" t="s">
         <v>219</v>
       </c>
@@ -1358,6 +1423,9 @@
       <c r="D18" t="s">
         <v>7</v>
       </c>
+      <c r="E18" s="3">
+        <v>29.07</v>
+      </c>
       <c r="F18" t="s">
         <v>220</v>
       </c>
@@ -1375,6 +1443,9 @@
       <c r="D19" t="s">
         <v>8</v>
       </c>
+      <c r="E19" s="3">
+        <v>6.43</v>
+      </c>
       <c r="F19" t="s">
         <v>221</v>
       </c>
@@ -1392,6 +1463,9 @@
       <c r="D20" t="s">
         <v>7</v>
       </c>
+      <c r="E20" s="3">
+        <v>6.88</v>
+      </c>
       <c r="F20" t="s">
         <v>222</v>
       </c>
@@ -1409,6 +1483,9 @@
       <c r="D21" t="s">
         <v>8</v>
       </c>
+      <c r="E21" s="3">
+        <v>6.19</v>
+      </c>
       <c r="F21" t="s">
         <v>223</v>
       </c>
@@ -1426,6 +1503,9 @@
       <c r="D22" t="s">
         <v>7</v>
       </c>
+      <c r="E22" s="3">
+        <v>17.73</v>
+      </c>
       <c r="F22" t="s">
         <v>224</v>
       </c>
@@ -1443,6 +1523,9 @@
       <c r="D23" t="s">
         <v>8</v>
       </c>
+      <c r="E23" s="3">
+        <v>8.36</v>
+      </c>
       <c r="F23" t="s">
         <v>196</v>
       </c>
@@ -1460,6 +1543,9 @@
       <c r="D24" t="s">
         <v>7</v>
       </c>
+      <c r="E24" s="3">
+        <v>25.64</v>
+      </c>
       <c r="F24" t="s">
         <v>225</v>
       </c>
@@ -1477,6 +1563,9 @@
       <c r="D25" t="s">
         <v>8</v>
       </c>
+      <c r="E25" s="3">
+        <v>3.87</v>
+      </c>
       <c r="F25" t="s">
         <v>226</v>
       </c>
@@ -1494,6 +1583,9 @@
       <c r="D26" t="s">
         <v>7</v>
       </c>
+      <c r="E26" s="3">
+        <v>8.56</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
@@ -1508,6 +1600,9 @@
       <c r="D27" t="s">
         <v>8</v>
       </c>
+      <c r="E27" s="3">
+        <v>7.47</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
@@ -1522,6 +1617,9 @@
       <c r="D28" t="s">
         <v>7</v>
       </c>
+      <c r="E28" s="3">
+        <v>10.130000000000001</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
@@ -1536,6 +1634,9 @@
       <c r="D29" t="s">
         <v>8</v>
       </c>
+      <c r="E29" s="3">
+        <v>3.04</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
@@ -1550,6 +1651,9 @@
       <c r="D30" t="s">
         <v>7</v>
       </c>
+      <c r="E30" s="3">
+        <v>13.89</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
@@ -1564,6 +1668,9 @@
       <c r="D31" t="s">
         <v>8</v>
       </c>
+      <c r="E31" s="3">
+        <v>4.8099999999999996</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
@@ -1578,8 +1685,11 @@
       <c r="D32" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="3">
+        <v>6.71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>45503</v>
       </c>
@@ -1592,8 +1702,11 @@
       <c r="D33" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="3">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>45503</v>
       </c>
@@ -1606,8 +1719,11 @@
       <c r="D34" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="3">
+        <v>16.72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>45503</v>
       </c>
@@ -1620,8 +1736,11 @@
       <c r="D35" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="3">
+        <v>5.94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>45503</v>
       </c>
@@ -1634,8 +1753,11 @@
       <c r="D36" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="3">
+        <v>6.78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>45503</v>
       </c>
@@ -1648,8 +1770,11 @@
       <c r="D37" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="3">
+        <v>3.13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>45504</v>
       </c>
@@ -1662,8 +1787,11 @@
       <c r="D38" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>45504</v>
       </c>
@@ -1676,8 +1804,11 @@
       <c r="D39" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>45504</v>
       </c>
@@ -1690,8 +1821,11 @@
       <c r="D40" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>45504</v>
       </c>
@@ -1704,8 +1838,11 @@
       <c r="D41" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>45504</v>
       </c>
@@ -1718,8 +1855,11 @@
       <c r="D42" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>45504</v>
       </c>
@@ -1732,8 +1872,11 @@
       <c r="D43" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>45504</v>
       </c>
@@ -1746,8 +1889,11 @@
       <c r="D44" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>45504</v>
       </c>
@@ -1760,8 +1906,11 @@
       <c r="D45" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45504</v>
       </c>
@@ -1774,8 +1923,11 @@
       <c r="D46" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45504</v>
       </c>
@@ -1788,8 +1940,11 @@
       <c r="D47" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>45504</v>
       </c>
@@ -1802,8 +1957,11 @@
       <c r="D48" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>45504</v>
       </c>
@@ -1816,8 +1974,11 @@
       <c r="D49" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>45505</v>
       </c>
@@ -1830,8 +1991,11 @@
       <c r="D50" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>45505</v>
       </c>
@@ -1844,8 +2008,11 @@
       <c r="D51" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>45505</v>
       </c>
@@ -1858,8 +2025,11 @@
       <c r="D52" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>45505</v>
       </c>
@@ -1872,8 +2042,11 @@
       <c r="D53" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>45505</v>
       </c>
@@ -1886,8 +2059,11 @@
       <c r="D54" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>45505</v>
       </c>
@@ -1900,8 +2076,11 @@
       <c r="D55" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>45505</v>
       </c>
@@ -1914,8 +2093,11 @@
       <c r="D56" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>45505</v>
       </c>
@@ -1928,8 +2110,11 @@
       <c r="D57" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>45505</v>
       </c>
@@ -1942,8 +2127,11 @@
       <c r="D58" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>45505</v>
       </c>
@@ -1956,8 +2144,11 @@
       <c r="D59" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>45505</v>
       </c>
@@ -1970,8 +2161,11 @@
       <c r="D60" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>45505</v>
       </c>
@@ -1984,8 +2178,11 @@
       <c r="D61" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>45510</v>
       </c>
@@ -1998,8 +2195,11 @@
       <c r="D62" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" s="3">
+        <v>-13.15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>45510</v>
       </c>
@@ -2012,8 +2212,11 @@
       <c r="D63" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" s="3">
+        <v>-21.84</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>45510</v>
       </c>
@@ -2026,8 +2229,11 @@
       <c r="D64" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" s="3">
+        <v>-22.38</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>45510</v>
       </c>
@@ -2040,8 +2246,11 @@
       <c r="D65" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" s="3">
+        <v>-32.200000000000003</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>45510</v>
       </c>
@@ -2054,8 +2263,11 @@
       <c r="D66" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" s="3">
+        <v>-46.55</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>45510</v>
       </c>
@@ -2068,8 +2280,11 @@
       <c r="D67" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" s="3">
+        <v>-33.79</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>45510</v>
       </c>
@@ -2082,8 +2297,11 @@
       <c r="D68" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" s="3">
+        <v>-3.27</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>45510</v>
       </c>
@@ -2096,8 +2314,11 @@
       <c r="D69" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" s="3">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>45510</v>
       </c>
@@ -2110,8 +2331,11 @@
       <c r="D70" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70" s="3">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>45510</v>
       </c>
@@ -2124,8 +2348,11 @@
       <c r="D71" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" s="3">
+        <v>3.77</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>45510</v>
       </c>
@@ -2138,8 +2365,11 @@
       <c r="D72" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72" s="3">
+        <v>5.94</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>45510</v>
       </c>
@@ -2152,8 +2382,11 @@
       <c r="D73" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73" s="3">
+        <v>2.2400000000000002</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>45510</v>
       </c>
@@ -2166,8 +2399,11 @@
       <c r="D74" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74" s="3">
+        <v>4.6399999999999997</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>45510</v>
       </c>
@@ -2180,8 +2416,11 @@
       <c r="D75" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75" s="3">
+        <v>1.64</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>45510</v>
       </c>
@@ -2194,8 +2433,11 @@
       <c r="D76" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76" s="3">
+        <v>8.6199999999999992</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>45510</v>
       </c>
@@ -2208,8 +2450,11 @@
       <c r="D77" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77" s="3">
+        <v>4.6100000000000003</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>45510</v>
       </c>
@@ -2222,8 +2467,11 @@
       <c r="D78" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78" s="3">
+        <v>7.47</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>45510</v>
       </c>
@@ -2236,8 +2484,11 @@
       <c r="D79" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79" s="3">
+        <v>7.43</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>45510</v>
       </c>
@@ -2250,8 +2501,11 @@
       <c r="D80" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80" s="3">
+        <v>5.61</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>45510</v>
       </c>
@@ -2264,8 +2518,11 @@
       <c r="D81" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81" s="3">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>45510</v>
       </c>
@@ -2278,8 +2535,11 @@
       <c r="D82" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82" s="3">
+        <v>2.3199999999999998</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>45510</v>
       </c>
@@ -2292,8 +2552,11 @@
       <c r="D83" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83" s="3">
+        <v>2.69</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>45510</v>
       </c>
@@ -2306,8 +2569,11 @@
       <c r="D84" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84" s="3">
+        <v>12.14</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>45510</v>
       </c>
@@ -2320,8 +2586,11 @@
       <c r="D85" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85" s="3">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>45510</v>
       </c>
@@ -2334,8 +2603,11 @@
       <c r="D86" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86" s="3">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>45510</v>
       </c>
@@ -2348,8 +2620,11 @@
       <c r="D87" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87" s="3">
+        <v>6.12</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>45510</v>
       </c>
@@ -2362,8 +2637,11 @@
       <c r="D88" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88" s="3">
+        <v>10.95</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>45510</v>
       </c>
@@ -2376,8 +2654,11 @@
       <c r="D89" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89" s="3">
+        <v>4.9400000000000004</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>45510</v>
       </c>
@@ -2390,8 +2671,11 @@
       <c r="D90" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90" s="3">
+        <v>8.52</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>45510</v>
       </c>
@@ -2404,8 +2688,11 @@
       <c r="D91" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91" s="3">
+        <v>6.61</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>45510</v>
       </c>
@@ -2418,8 +2705,11 @@
       <c r="D92" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92" s="3">
+        <v>7.66</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>45510</v>
       </c>
@@ -2432,8 +2722,11 @@
       <c r="D93" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93" s="3">
+        <v>5.35</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>45510</v>
       </c>
@@ -2446,8 +2739,11 @@
       <c r="D94" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94" s="3">
+        <v>6.96</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>45510</v>
       </c>
@@ -2460,8 +2756,11 @@
       <c r="D95" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95" s="3">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>45510</v>
       </c>
@@ -2474,8 +2773,11 @@
       <c r="D96" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96" s="3">
+        <v>8.18</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>45510</v>
       </c>
@@ -2488,8 +2790,11 @@
       <c r="D97" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97" s="3">
+        <v>5.26</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>45512</v>
       </c>
@@ -2502,8 +2807,11 @@
       <c r="D98" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98" s="3">
+        <v>-16.52</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>45512</v>
       </c>
@@ -2516,8 +2824,11 @@
       <c r="D99" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99" s="3">
+        <v>-9.83</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>45512</v>
       </c>
@@ -2530,8 +2841,11 @@
       <c r="D100" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100" s="3">
+        <v>3.18</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>45512</v>
       </c>
@@ -2544,8 +2858,11 @@
       <c r="D101" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101" s="3">
+        <v>-7.8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>45512</v>
       </c>
@@ -2558,8 +2875,11 @@
       <c r="D102" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102" s="3">
+        <v>-13.37</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>45512</v>
       </c>
@@ -2572,8 +2892,11 @@
       <c r="D103" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103" s="3">
+        <v>-17.93</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>45512</v>
       </c>
@@ -2586,8 +2909,11 @@
       <c r="D104" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104" s="3">
+        <v>16.27</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>45512</v>
       </c>
@@ -2600,8 +2926,11 @@
       <c r="D105" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105" s="3">
+        <v>3.37</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>45512</v>
       </c>
@@ -2614,8 +2943,11 @@
       <c r="D106" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E106" s="3">
+        <v>11.31</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>45512</v>
       </c>
@@ -2628,8 +2960,11 @@
       <c r="D107" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E107" s="2">
+        <v>7.91</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>45512</v>
       </c>
@@ -2642,8 +2977,11 @@
       <c r="D108" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E108" s="3">
+        <v>4.74</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>45512</v>
       </c>
@@ -2656,8 +2994,11 @@
       <c r="D109" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>45512</v>
       </c>
@@ -2670,8 +3011,11 @@
       <c r="D110" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E110" s="3">
+        <v>28.79</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>45512</v>
       </c>
@@ -2684,8 +3028,11 @@
       <c r="D111" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E111" s="3">
+        <v>9.07</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>45512</v>
       </c>
@@ -2698,8 +3045,11 @@
       <c r="D112" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E112" s="3">
+        <v>11.23</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>45512</v>
       </c>
@@ -2712,8 +3062,11 @@
       <c r="D113" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E113" s="3">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>45512</v>
       </c>
@@ -2726,8 +3079,11 @@
       <c r="D114" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E114" s="3">
+        <v>8.67</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>45512</v>
       </c>
@@ -2740,8 +3096,11 @@
       <c r="D115" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E115" s="3">
+        <v>6.06</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>45512</v>
       </c>
@@ -2754,8 +3113,11 @@
       <c r="D116" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E116" s="3">
+        <v>22.17</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>45512</v>
       </c>
@@ -2768,8 +3130,11 @@
       <c r="D117" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E117" s="3">
+        <v>27.84</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>45512</v>
       </c>
@@ -2782,8 +3147,11 @@
       <c r="D118" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E118" s="3">
+        <v>13.62</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>45512</v>
       </c>
@@ -2796,8 +3164,11 @@
       <c r="D119" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E119" s="3">
+        <v>5.35</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>45512</v>
       </c>
@@ -2810,8 +3181,11 @@
       <c r="D120" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E120" s="3">
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>45512</v>
       </c>
@@ -2824,8 +3198,11 @@
       <c r="D121" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E121" s="3">
+        <v>4.08</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>45517</v>
       </c>
@@ -2838,8 +3215,11 @@
       <c r="D122" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E122" s="3">
+        <v>5.67</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>45517</v>
       </c>
@@ -2852,8 +3232,11 @@
       <c r="D123" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E123" s="3">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>45517</v>
       </c>
@@ -2866,8 +3249,11 @@
       <c r="D124" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E124" s="3">
+        <v>-1.52</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>45517</v>
       </c>
@@ -2880,8 +3266,11 @@
       <c r="D125" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E125" s="3">
+        <v>-1.61</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>45517</v>
       </c>
@@ -2894,8 +3283,11 @@
       <c r="D126" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E126" s="3">
+        <v>-5.89</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>45517</v>
       </c>
@@ -2908,8 +3300,11 @@
       <c r="D127" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E127" s="3">
+        <v>-7.89</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>45517</v>
       </c>
@@ -2922,8 +3317,11 @@
       <c r="D128" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E128" s="3">
+        <v>-6.82</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>45517</v>
       </c>
@@ -2936,8 +3334,11 @@
       <c r="D129" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E129" s="3">
+        <v>-8.2100000000000009</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>45517</v>
       </c>
@@ -2950,8 +3351,11 @@
       <c r="D130" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E130" s="3">
+        <v>-1.46</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>45517</v>
       </c>
@@ -2964,8 +3368,11 @@
       <c r="D131" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E131" s="3">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>45517</v>
       </c>
@@ -2978,8 +3385,11 @@
       <c r="D132" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E132" s="3">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>45517</v>
       </c>
@@ -2992,8 +3402,11 @@
       <c r="D133" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E133" s="3">
+        <v>2.68</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>45517</v>
       </c>
@@ -3006,8 +3419,11 @@
       <c r="D134" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E134" s="3">
+        <v>6.47</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>45517</v>
       </c>
@@ -3020,8 +3436,11 @@
       <c r="D135" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E135" s="3">
+        <v>6.97</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>45517</v>
       </c>
@@ -3034,8 +3453,11 @@
       <c r="D136" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E136" s="3">
+        <v>7.18</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>45517</v>
       </c>
@@ -3048,8 +3470,11 @@
       <c r="D137" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E137" s="3">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>45517</v>
       </c>
@@ -3062,8 +3487,11 @@
       <c r="D138" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E138" s="3">
+        <v>4.8099999999999996</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>45517</v>
       </c>
@@ -3076,8 +3504,11 @@
       <c r="D139" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E139" s="3">
+        <v>2.5299999999999998</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>45517</v>
       </c>
@@ -3090,8 +3521,11 @@
       <c r="D140" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E140" s="3">
+        <v>13.72</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>45517</v>
       </c>
@@ -3104,8 +3538,11 @@
       <c r="D141" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E141" s="3">
+        <v>15.65</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>45517</v>
       </c>
@@ -3118,8 +3555,11 @@
       <c r="D142" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E142" s="3">
+        <v>8.8800000000000008</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>45517</v>
       </c>
@@ -3132,8 +3572,11 @@
       <c r="D143" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E143" s="3">
+        <v>6.88</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>45517</v>
       </c>
@@ -3146,8 +3589,11 @@
       <c r="D144" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E144" s="3">
+        <v>13.77</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>45517</v>
       </c>
@@ -3160,8 +3606,11 @@
       <c r="D145" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E145" s="3">
+        <v>4.59</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>45524</v>
       </c>
@@ -3174,8 +3623,11 @@
       <c r="D146" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E146" s="3">
+        <v>2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>45524</v>
       </c>
@@ -3188,8 +3640,11 @@
       <c r="D147" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E147" s="3">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>45524</v>
       </c>
@@ -3202,8 +3657,11 @@
       <c r="D148" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E148" s="3">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>45524</v>
       </c>
@@ -3216,8 +3674,11 @@
       <c r="D149" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E149" s="3">
+        <v>5.23</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>45524</v>
       </c>
@@ -3230,8 +3691,11 @@
       <c r="D150" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E150" s="3">
+        <v>3.81</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>45524</v>
       </c>
@@ -3244,8 +3708,11 @@
       <c r="D151" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E151" s="3">
+        <v>5.27</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>45524</v>
       </c>
@@ -3258,8 +3725,11 @@
       <c r="D152" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E152" s="3">
+        <v>3.13</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>45524</v>
       </c>
@@ -3272,8 +3742,11 @@
       <c r="D153" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E153" s="3">
+        <v>4.24</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>45524</v>
       </c>
@@ -3286,8 +3759,11 @@
       <c r="D154" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E154" s="3">
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>45524</v>
       </c>
@@ -3300,8 +3776,11 @@
       <c r="D155" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E155" s="3">
+        <v>3.36</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>45524</v>
       </c>
@@ -3314,8 +3793,11 @@
       <c r="D156" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E156" s="3">
+        <v>6.37</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>45524</v>
       </c>
@@ -3328,8 +3810,11 @@
       <c r="D157" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E157" s="3">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>45524</v>
       </c>
@@ -3342,8 +3827,11 @@
       <c r="D158" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E158" s="3">
+        <v>-2.34</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>45524</v>
       </c>
@@ -3356,8 +3844,11 @@
       <c r="D159" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E159" s="3">
+        <v>-1.67</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>45524</v>
       </c>
@@ -3370,8 +3861,11 @@
       <c r="D160" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E160" s="3">
+        <v>6.28</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>45524</v>
       </c>
@@ -3384,8 +3878,11 @@
       <c r="D161" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E161" s="3">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>45524</v>
       </c>
@@ -3398,8 +3895,11 @@
       <c r="D162" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E162" s="3">
+        <v>8.01</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>45524</v>
       </c>
@@ -3412,8 +3912,11 @@
       <c r="D163" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E163" s="3">
+        <v>1.66</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>45524</v>
       </c>
@@ -3426,8 +3929,11 @@
       <c r="D164" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E164" s="3">
+        <v>7.61</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>45524</v>
       </c>
@@ -3440,8 +3946,11 @@
       <c r="D165" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E165" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>45524</v>
       </c>
@@ -3454,8 +3963,11 @@
       <c r="D166" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E166" s="3">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>45524</v>
       </c>
@@ -3468,8 +3980,11 @@
       <c r="D167" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E167" s="3">
+        <v>-1.47</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>45524</v>
       </c>
@@ -3482,8 +3997,11 @@
       <c r="D168" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E168" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>45524</v>
       </c>
@@ -3496,8 +4014,11 @@
       <c r="D169" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E169" s="3">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>45526</v>
       </c>
@@ -3510,8 +4031,11 @@
       <c r="D170" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E170" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>45526</v>
       </c>
@@ -3524,8 +4048,11 @@
       <c r="D171" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E171" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>45526</v>
       </c>
@@ -3538,8 +4065,11 @@
       <c r="D172" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E172" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>45526</v>
       </c>
@@ -3552,8 +4082,11 @@
       <c r="D173" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E173" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>45526</v>
       </c>
@@ -3566,8 +4099,11 @@
       <c r="D174" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E174" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>45526</v>
       </c>
@@ -3580,8 +4116,11 @@
       <c r="D175" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E175" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>45526</v>
       </c>
@@ -3594,8 +4133,11 @@
       <c r="D176" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E176" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>45526</v>
       </c>
@@ -3608,8 +4150,11 @@
       <c r="D177" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E177" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>45526</v>
       </c>
@@ -3622,8 +4167,11 @@
       <c r="D178" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E178" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>45526</v>
       </c>
@@ -3636,8 +4184,11 @@
       <c r="D179" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E179" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>45526</v>
       </c>
@@ -3650,8 +4201,11 @@
       <c r="D180" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E180" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>45526</v>
       </c>
@@ -3664,8 +4218,11 @@
       <c r="D181" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E181" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>45531</v>
       </c>
@@ -3678,8 +4235,11 @@
       <c r="D182" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E182" s="3">
+        <v>8.8699999999999992</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>45531</v>
       </c>
@@ -3692,8 +4252,11 @@
       <c r="D183" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E183" s="3">
+        <v>4.66</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>45531</v>
       </c>
@@ -3706,8 +4269,11 @@
       <c r="D184" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E184" s="3">
+        <v>8.68</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>45531</v>
       </c>
@@ -3720,8 +4286,11 @@
       <c r="D185" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E185" s="3">
+        <v>6.47</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>45531</v>
       </c>
@@ -3734,8 +4303,11 @@
       <c r="D186" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E186" s="3">
+        <v>7.61</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>45531</v>
       </c>
@@ -3748,8 +4320,11 @@
       <c r="D187" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E187" s="3">
+        <v>7.42</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>45531</v>
       </c>
@@ -3762,8 +4337,11 @@
       <c r="D188" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E188" s="3">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>45531</v>
       </c>
@@ -3776,8 +4354,11 @@
       <c r="D189" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E189" s="3">
+        <v>2.16</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>45531</v>
       </c>
@@ -3790,8 +4371,11 @@
       <c r="D190" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E190" s="3">
+        <v>4.1100000000000003</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>45531</v>
       </c>
@@ -3804,8 +4388,11 @@
       <c r="D191" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E191" s="3">
+        <v>3.66</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>45531</v>
       </c>
@@ -3818,8 +4405,11 @@
       <c r="D192" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E192" s="3">
+        <v>13.26</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>45531</v>
       </c>
@@ -3832,8 +4422,11 @@
       <c r="D193" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E193" s="3">
+        <v>7.27</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>45538</v>
       </c>
@@ -3846,8 +4439,11 @@
       <c r="D194" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E194" s="3">
+        <v>14.98</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>45538</v>
       </c>
@@ -3860,8 +4456,11 @@
       <c r="D195" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E195" s="5">
+        <v>-3.74</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>45538</v>
       </c>
@@ -3874,8 +4473,11 @@
       <c r="D196" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E196" s="3">
+        <v>6.61</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>45538</v>
       </c>
@@ -3888,8 +4490,11 @@
       <c r="D197" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E197" s="5">
+        <v>-2.5499999999999998</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>45538</v>
       </c>
@@ -3902,8 +4507,11 @@
       <c r="D198" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E198" s="3">
+        <v>15.81</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>45538</v>
       </c>
@@ -3916,8 +4524,11 @@
       <c r="D199" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E199" s="5">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>45538</v>
       </c>
@@ -3930,8 +4541,11 @@
       <c r="D200" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E200" s="3">
+        <v>4.26</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>45538</v>
       </c>
@@ -3944,8 +4558,11 @@
       <c r="D201" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E201" s="5">
+        <v>-4.9800000000000004</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>45538</v>
       </c>
@@ -3958,8 +4575,11 @@
       <c r="D202" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E202" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>45538</v>
       </c>
@@ -3972,8 +4592,11 @@
       <c r="D203" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E203" s="5">
+        <v>-2.99</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>45538</v>
       </c>
@@ -3986,8 +4609,11 @@
       <c r="D204" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E204" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>45538</v>
       </c>
@@ -4000,8 +4626,11 @@
       <c r="D205" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E205" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>45587</v>
       </c>
@@ -4014,8 +4643,11 @@
       <c r="D206" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E206" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>45587</v>
       </c>
@@ -4028,8 +4660,11 @@
       <c r="D207" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E207" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>45587</v>
       </c>
@@ -4042,8 +4677,11 @@
       <c r="D208" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E208" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>45587</v>
       </c>
@@ -4056,8 +4694,11 @@
       <c r="D209" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E209" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>45587</v>
       </c>
@@ -4070,8 +4711,11 @@
       <c r="D210" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E210" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>45587</v>
       </c>
@@ -4084,8 +4728,11 @@
       <c r="D211" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E211" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>45587</v>
       </c>
@@ -4098,8 +4745,11 @@
       <c r="D212" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E212" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>45587</v>
       </c>
@@ -4112,8 +4762,11 @@
       <c r="D213" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E213" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>45587</v>
       </c>
@@ -4126,8 +4779,11 @@
       <c r="D214" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E214" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>45587</v>
       </c>
@@ -4140,8 +4796,11 @@
       <c r="D215" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E215" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>45587</v>
       </c>
@@ -4154,8 +4813,11 @@
       <c r="D216" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E216" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>45587</v>
       </c>
@@ -4168,8 +4830,11 @@
       <c r="D217" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E217" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>45587</v>
       </c>
@@ -4182,8 +4847,11 @@
       <c r="D218" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E218" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>45587</v>
       </c>
@@ -4196,8 +4864,11 @@
       <c r="D219" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E219" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>45587</v>
       </c>
@@ -4210,8 +4881,11 @@
       <c r="D220" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E220" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>45587</v>
       </c>
@@ -4224,8 +4898,11 @@
       <c r="D221" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E221" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>45587</v>
       </c>
@@ -4238,8 +4915,11 @@
       <c r="D222" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E222" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>45587</v>
       </c>
@@ -4252,8 +4932,11 @@
       <c r="D223" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E223" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>45587</v>
       </c>
@@ -4266,8 +4949,11 @@
       <c r="D224" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E224" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>45587</v>
       </c>
@@ -4280,8 +4966,11 @@
       <c r="D225" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E225" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>45587</v>
       </c>
@@ -4294,8 +4983,11 @@
       <c r="D226" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E226" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>45587</v>
       </c>
@@ -4308,8 +5000,11 @@
       <c r="D227" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E227" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>45587</v>
       </c>
@@ -4322,8 +5017,11 @@
       <c r="D228" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E228" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>45587</v>
       </c>
@@ -4336,8 +5034,11 @@
       <c r="D229" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E229" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>45595</v>
       </c>
@@ -4350,8 +5051,11 @@
       <c r="D230" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E230" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>45595</v>
       </c>
@@ -4364,8 +5068,11 @@
       <c r="D231" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E231" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>45595</v>
       </c>
@@ -4378,8 +5085,11 @@
       <c r="D232" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E232" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>45595</v>
       </c>
@@ -4392,8 +5102,11 @@
       <c r="D233" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E233" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>45595</v>
       </c>
@@ -4406,8 +5119,11 @@
       <c r="D234" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E234" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>45595</v>
       </c>
@@ -4420,8 +5136,11 @@
       <c r="D235" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E235" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>45595</v>
       </c>
@@ -4434,8 +5153,11 @@
       <c r="D236" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E236" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>45595</v>
       </c>
@@ -4448,8 +5170,11 @@
       <c r="D237" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E237" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>45595</v>
       </c>
@@ -4462,8 +5187,11 @@
       <c r="D238" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E238" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>45595</v>
       </c>
@@ -4476,8 +5204,11 @@
       <c r="D239" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E239" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>45595</v>
       </c>
@@ -4490,8 +5221,11 @@
       <c r="D240" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E240" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>45595</v>
       </c>
@@ -4504,8 +5238,11 @@
       <c r="D241" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E241" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>45595</v>
       </c>
@@ -4518,8 +5255,11 @@
       <c r="D242" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E242" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>45595</v>
       </c>
@@ -4532,8 +5272,11 @@
       <c r="D243" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E243" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>45595</v>
       </c>
@@ -4546,8 +5289,11 @@
       <c r="D244" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E244" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>45595</v>
       </c>
@@ -4560,8 +5306,11 @@
       <c r="D245" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E245" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>45595</v>
       </c>
@@ -4574,8 +5323,11 @@
       <c r="D246" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E246" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>45595</v>
       </c>
@@ -4588,8 +5340,11 @@
       <c r="D247" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E247" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>45595</v>
       </c>
@@ -4602,8 +5357,11 @@
       <c r="D248" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E248" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>45595</v>
       </c>
@@ -4616,8 +5374,11 @@
       <c r="D249" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E249" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>45595</v>
       </c>
@@ -4630,8 +5391,11 @@
       <c r="D250" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E250" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>45595</v>
       </c>
@@ -4644,8 +5408,11 @@
       <c r="D251" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E251" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>45595</v>
       </c>
@@ -4658,8 +5425,11 @@
       <c r="D252" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E252" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>45595</v>
       </c>
@@ -4672,8 +5442,11 @@
       <c r="D253" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E253" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>45615</v>
       </c>
@@ -4686,8 +5459,11 @@
       <c r="D254" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E254" s="3">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>45615</v>
       </c>
@@ -4700,8 +5476,11 @@
       <c r="D255" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E255" s="3">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>45615</v>
       </c>
@@ -4714,8 +5493,11 @@
       <c r="D256" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E256" s="3">
+        <v>6.83</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>45615</v>
       </c>
@@ -4728,8 +5510,11 @@
       <c r="D257" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E257" s="3">
+        <v>3.18</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>45615</v>
       </c>
@@ -4742,8 +5527,11 @@
       <c r="D258" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E258" s="3">
+        <v>6.21</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>45615</v>
       </c>
@@ -4756,8 +5544,11 @@
       <c r="D259" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E259" s="3">
+        <v>2.02</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>45615</v>
       </c>
@@ -4770,8 +5561,11 @@
       <c r="D260" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E260" s="3">
+        <v>2.27</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>45615</v>
       </c>
@@ -4784,8 +5578,11 @@
       <c r="D261" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E261" s="3">
+        <v>2.16</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>45615</v>
       </c>
@@ -4798,8 +5595,11 @@
       <c r="D262" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E262" s="3">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>45615</v>
       </c>
@@ -4812,8 +5612,11 @@
       <c r="D263" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E263" s="3">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>45615</v>
       </c>
@@ -4826,8 +5629,11 @@
       <c r="D264" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E264" s="3">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>45621</v>
       </c>
@@ -4840,8 +5646,11 @@
       <c r="D265" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E265" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>45621</v>
       </c>
@@ -4854,8 +5663,11 @@
       <c r="D266" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E266" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>45621</v>
       </c>
@@ -4868,8 +5680,11 @@
       <c r="D267" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E267" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>45621</v>
       </c>
@@ -4882,8 +5697,11 @@
       <c r="D268" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E268" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>45621</v>
       </c>
@@ -4896,8 +5714,11 @@
       <c r="D269" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E269" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>45621</v>
       </c>
@@ -4910,8 +5731,11 @@
       <c r="D270" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E270" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>45621</v>
       </c>
@@ -4924,8 +5748,11 @@
       <c r="D271" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E271" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>45621</v>
       </c>
@@ -4937,6 +5764,9 @@
       </c>
       <c r="D272" t="s">
         <v>7</v>
+      </c>
+      <c r="E272" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
@@ -4952,6 +5782,9 @@
       <c r="D273" t="s">
         <v>7</v>
       </c>
+      <c r="E273" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
@@ -4966,6 +5799,9 @@
       <c r="D274" t="s">
         <v>7</v>
       </c>
+      <c r="E274" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
@@ -4980,6 +5816,9 @@
       <c r="D275" t="s">
         <v>7</v>
       </c>
+      <c r="E275" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
@@ -4994,6 +5833,9 @@
       <c r="D276" t="s">
         <v>7</v>
       </c>
+      <c r="E276" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
@@ -5008,7 +5850,7 @@
       <c r="D277" t="s">
         <v>7</v>
       </c>
-      <c r="E277" t="s">
+      <c r="E277" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -5025,7 +5867,7 @@
       <c r="D278" t="s">
         <v>7</v>
       </c>
-      <c r="E278" t="s">
+      <c r="E278" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -5042,7 +5884,7 @@
       <c r="D279" t="s">
         <v>7</v>
       </c>
-      <c r="E279" t="s">
+      <c r="E279" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -5059,7 +5901,7 @@
       <c r="D280" t="s">
         <v>7</v>
       </c>
-      <c r="E280" t="s">
+      <c r="E280" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -5076,7 +5918,7 @@
       <c r="D281" t="s">
         <v>7</v>
       </c>
-      <c r="E281" t="s">
+      <c r="E281" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -5093,7 +5935,7 @@
       <c r="D282" t="s">
         <v>7</v>
       </c>
-      <c r="E282" t="s">
+      <c r="E282" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -5110,7 +5952,7 @@
       <c r="D283" t="s">
         <v>7</v>
       </c>
-      <c r="E283" t="s">
+      <c r="E283" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -5127,7 +5969,7 @@
       <c r="D284" t="s">
         <v>7</v>
       </c>
-      <c r="E284" t="s">
+      <c r="E284" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -5144,7 +5986,7 @@
       <c r="D285" t="s">
         <v>7</v>
       </c>
-      <c r="E285" t="s">
+      <c r="E285" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -5161,7 +6003,7 @@
       <c r="D286" t="s">
         <v>7</v>
       </c>
-      <c r="E286" t="s">
+      <c r="E286" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -5178,7 +6020,7 @@
       <c r="D287" t="s">
         <v>7</v>
       </c>
-      <c r="E287" t="s">
+      <c r="E287" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -5195,11 +6037,11 @@
       <c r="D288" t="s">
         <v>7</v>
       </c>
-      <c r="E288" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E288" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>45649</v>
       </c>
@@ -5216,7 +6058,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>45649</v>
       </c>
@@ -5233,7 +6075,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>45649</v>
       </c>
@@ -5250,7 +6092,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>45649</v>
       </c>
@@ -5267,7 +6109,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>45649</v>
       </c>
@@ -5284,7 +6126,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>45649</v>
       </c>
@@ -5301,7 +6143,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>45649</v>
       </c>
@@ -5318,7 +6160,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>45649</v>
       </c>
@@ -5335,7 +6177,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>45649</v>
       </c>
@@ -5352,7 +6194,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>45649</v>
       </c>
@@ -5369,7 +6211,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>45649</v>
       </c>
@@ -5386,7 +6228,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>45649</v>
       </c>
@@ -5403,7 +6245,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>45659</v>
       </c>
@@ -5419,8 +6261,11 @@
       <c r="E301">
         <v>15.31</v>
       </c>
-    </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F301" s="6">
+        <v>13.75</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>45659</v>
       </c>
@@ -5436,8 +6281,11 @@
       <c r="E302">
         <v>12.98</v>
       </c>
-    </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F302" s="6">
+        <v>11.63</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>45659</v>
       </c>
@@ -5453,8 +6301,11 @@
       <c r="E303">
         <v>18.920000000000002</v>
       </c>
-    </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F303" s="6">
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>45659</v>
       </c>
@@ -5470,8 +6321,11 @@
       <c r="E304" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F304" s="6">
+        <v>8.44</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>45659</v>
       </c>
@@ -5487,8 +6341,11 @@
       <c r="E305" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F305" s="6">
+        <v>8.91</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>45659</v>
       </c>
@@ -5504,8 +6361,11 @@
       <c r="E306">
         <v>11.92</v>
       </c>
-    </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F306" s="6">
+        <v>11.09</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>45659</v>
       </c>
@@ -5521,8 +6381,11 @@
       <c r="E307">
         <v>13.77</v>
       </c>
-    </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F307" s="6">
+        <v>20.59</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <v>45659</v>
       </c>
@@ -5538,8 +6401,11 @@
       <c r="E308">
         <v>12.77</v>
       </c>
-    </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F308" s="6">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>45659</v>
       </c>
@@ -5555,8 +6421,11 @@
       <c r="E309">
         <v>11.13</v>
       </c>
-    </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F309" s="6">
+        <v>12.27</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <v>45659</v>
       </c>
@@ -5572,8 +6441,11 @@
       <c r="E310">
         <v>17.309999999999999</v>
       </c>
-    </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F310" s="6">
+        <v>9.86</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <v>45659</v>
       </c>
@@ -5589,8 +6461,11 @@
       <c r="E311">
         <v>4.09</v>
       </c>
-    </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F311" s="6">
+        <v>2.98</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <v>45659</v>
       </c>
@@ -5606,8 +6481,11 @@
       <c r="E312">
         <v>7.15</v>
       </c>
-    </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F312" s="6">
+        <v>5.46</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>45665</v>
       </c>
@@ -5624,7 +6502,7 @@
         <v>5.51</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
         <v>45665</v>
       </c>
@@ -5641,7 +6519,7 @@
         <v>4.21</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
         <v>45665</v>
       </c>
@@ -5658,7 +6536,7 @@
         <v>4.46</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
         <v>45665</v>
       </c>
@@ -5675,7 +6553,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
         <v>45665</v>
       </c>
@@ -5692,7 +6570,7 @@
         <v>4.12</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
         <v>45673</v>
       </c>
@@ -5709,7 +6587,7 @@
         <v>28.78</v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
         <v>45673</v>
       </c>
@@ -5726,7 +6604,7 @@
         <v>33.17</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
         <v>45673</v>
       </c>

</xml_diff>